<commit_message>
added all fields in Match to required
</commit_message>
<xml_diff>
--- a/Data/Excel/Matches-Full-Data - Testing.xlsx
+++ b/Data/Excel/Matches-Full-Data - Testing.xlsx
@@ -28,9 +28,6 @@
     <t>Qatar Open</t>
   </si>
   <si>
-    <t>Final</t>
-  </si>
-  <si>
     <t>Tomas Berdych</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Chennai Open</t>
   </si>
   <si>
-    <t>Semi Final</t>
-  </si>
-  <si>
     <t>Grigor Dimitrov</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>Auckland Open</t>
   </si>
   <si>
-    <t>R-16</t>
-  </si>
-  <si>
     <t>Milos Raonic</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
     <t>Sydney International</t>
   </si>
   <si>
-    <t>Quarter Final</t>
-  </si>
-  <si>
     <t>Roger Federer</t>
   </si>
   <si>
@@ -116,6 +104,18 @@
   </si>
   <si>
     <t>Round</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>QF</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,7 +444,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,22 +462,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -505,19 +505,19 @@
         <v>42742</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -525,19 +525,19 @@
         <v>42743</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,16 +548,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -565,19 +565,19 @@
         <v>42749</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -585,19 +585,19 @@
         <v>42758</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -605,19 +605,19 @@
         <v>42806</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>